<commit_message>
Ajout amélioration personnage + arme et début equipement
</commit_message>
<xml_diff>
--- a/sources/Outiles/StatsPersonnages.xlsx
+++ b/sources/Outiles/StatsPersonnages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat_wfpn4na\Documents\GitHub\Jeu-Dzarian-Miniquoinquoin\Outiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat_wfpn4na\Documents\GitHub\Jeu-Dzarian-Miniquoinquoin\sources\Outiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{83A7DB04-9DC0-4EA2-9706-4E2E017FE603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26BC8925-F482-48AD-AAC3-F3495D3F1867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1140" windowWidth="21600" windowHeight="15435" xr2:uid="{26D64052-F692-4786-847A-089B52D9574B}"/>
+    <workbookView xWindow="24540" yWindow="2040" windowWidth="21600" windowHeight="15435" xr2:uid="{26D64052-F692-4786-847A-089B52D9574B}"/>
   </bookViews>
   <sheets>
     <sheet name="StatsPersonnages" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="57">
   <si>
     <t>Personages</t>
   </si>
@@ -700,7 +700,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -838,8 +838,8 @@
       <c r="I3" s="3">
         <v>0</v>
       </c>
-      <c r="J3" s="3">
-        <v>0</v>
+      <c r="J3" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="K3" s="3">
         <v>500</v>
@@ -853,8 +853,8 @@
       <c r="N3" s="3">
         <v>0</v>
       </c>
-      <c r="O3" s="3">
-        <v>0</v>
+      <c r="O3" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="P3" s="3">
         <v>100</v>
@@ -940,8 +940,8 @@
       <c r="I5" s="3">
         <v>0</v>
       </c>
-      <c r="J5" s="3">
-        <v>0</v>
+      <c r="J5" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="K5" s="3">
         <v>700</v>
@@ -955,8 +955,8 @@
       <c r="N5" s="3">
         <v>0</v>
       </c>
-      <c r="O5" s="3">
-        <v>0</v>
+      <c r="O5" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="P5" s="3">
         <v>200</v>
@@ -1042,8 +1042,8 @@
       <c r="I7" s="3">
         <v>0</v>
       </c>
-      <c r="J7" s="3">
-        <v>0</v>
+      <c r="J7" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="K7" s="3">
         <v>800</v>
@@ -1057,8 +1057,8 @@
       <c r="N7" s="3">
         <v>0</v>
       </c>
-      <c r="O7" s="3">
-        <v>0</v>
+      <c r="O7" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="P7" s="3">
         <v>150</v>
@@ -1144,8 +1144,8 @@
       <c r="I9" s="3">
         <v>0</v>
       </c>
-      <c r="J9" s="3">
-        <v>0</v>
+      <c r="J9" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="K9" s="3">
         <v>1000</v>
@@ -1159,8 +1159,8 @@
       <c r="N9" s="3">
         <v>0</v>
       </c>
-      <c r="O9" s="3">
-        <v>0</v>
+      <c r="O9" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="P9" s="3">
         <v>1000</v>
@@ -1246,8 +1246,8 @@
       <c r="I11" s="3">
         <v>0</v>
       </c>
-      <c r="J11" s="3">
-        <v>0</v>
+      <c r="J11" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="K11" s="3">
         <v>600</v>
@@ -1261,8 +1261,8 @@
       <c r="N11" s="3">
         <v>0</v>
       </c>
-      <c r="O11" s="3">
-        <v>0</v>
+      <c r="O11" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="P11" s="3">
         <v>1000</v>
@@ -1348,8 +1348,8 @@
       <c r="I13" s="3">
         <v>0</v>
       </c>
-      <c r="J13" s="3">
-        <v>0</v>
+      <c r="J13" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="K13" s="3">
         <v>2500</v>
@@ -1363,8 +1363,8 @@
       <c r="N13" s="3">
         <v>0</v>
       </c>
-      <c r="O13" s="3">
-        <v>0</v>
+      <c r="O13" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="P13" s="3">
         <v>2500</v>
@@ -1450,8 +1450,8 @@
       <c r="I15" s="3">
         <v>0</v>
       </c>
-      <c r="J15" s="3">
-        <v>0</v>
+      <c r="J15" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="K15" s="3">
         <v>2000</v>
@@ -1465,8 +1465,8 @@
       <c r="N15" s="3">
         <v>0</v>
       </c>
-      <c r="O15" s="3">
-        <v>0</v>
+      <c r="O15" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="P15" s="3">
         <v>150</v>
@@ -1552,8 +1552,8 @@
       <c r="I17" s="3">
         <v>0</v>
       </c>
-      <c r="J17" s="3">
-        <v>0</v>
+      <c r="J17" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="K17" s="3">
         <v>5000</v>
@@ -1567,8 +1567,8 @@
       <c r="N17" s="3">
         <v>0</v>
       </c>
-      <c r="O17" s="3">
-        <v>0</v>
+      <c r="O17" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="P17" s="3">
         <v>9999</v>

</xml_diff>